<commit_message>
moved to new income process, seems to be working with standard flow costs. Next step is to try rebalancing costs, which is more unstable or sensitive
</commit_message>
<xml_diff>
--- a/output/run1_table.xlsx
+++ b/output/run1_table.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="1015">
   <si>
     <t>Row</t>
   </si>
@@ -445,6 +445,2616 @@
   </si>
   <si>
     <t>iy=1, kappa2=0.5</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>unnamed</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>iy=1, kappa2=0.25</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>iy=1, kappa2=0.25</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>iy=1, kappa2=0.25</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>iy=1, kappa2=0.25</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>iy=1, kappa2=0.25</t>
   </si>
   <si>
     <t>cont_a, no meas err</t>
@@ -468,7 +3078,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -477,13 +3087,25 @@
       <diagonal/>
     </border>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,567 +3124,567 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>870</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>142</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>871</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>143</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>872</v>
       </c>
       <c r="B3" s="0">
-        <v>8.8635007362964036</v>
+        <v>11.10478787236034</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>873</v>
       </c>
       <c r="B4" s="0">
-        <v>23.958357281141744</v>
+        <v>26.937285645146559</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>874</v>
       </c>
       <c r="B5" s="0">
-        <v>0.98019867330675525</v>
+        <v>0.96932819366254985</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>5</v>
+        <v>875</v>
       </c>
       <c r="B6" s="0"/>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>6</v>
+        <v>876</v>
       </c>
       <c r="B7" s="0">
-        <v>1.0691087245941162</v>
+        <v>1.0991047620773315</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>7</v>
+        <v>877</v>
       </c>
       <c r="B8" s="0">
-        <v>0.77865374088287354</v>
+        <v>0.803355872631073</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>8</v>
+        <v>878</v>
       </c>
       <c r="B9" s="0">
-        <v>0.77865374088287354</v>
+        <v>0.803355872631073</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>9</v>
+        <v>879</v>
       </c>
       <c r="B10" s="0"/>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>10</v>
+        <v>880</v>
       </c>
       <c r="B11" s="0">
-        <v>0.99649897438388102</v>
+        <v>4.1000312263037682</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>11</v>
+        <v>881</v>
       </c>
       <c r="B12" s="0">
-        <v>0.69295005152796185</v>
+        <v>0.41403322321604691</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>12</v>
+        <v>882</v>
       </c>
       <c r="B13" s="0">
-        <v>0.24704698512579756</v>
+        <v>0.32301171297246056</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>13</v>
+        <v>883</v>
       </c>
       <c r="B14" s="0">
-        <v>0.15095320303095686</v>
+        <v>0.049999982106113131</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>14</v>
+        <v>884</v>
       </c>
       <c r="B15" s="0">
-        <v>0.18895812189976166</v>
+        <v>0.17916849052428613</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>15</v>
+        <v>885</v>
       </c>
       <c r="B16" s="0">
-        <v>0.059333507258861745</v>
+        <v>0.079788190309264595</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>16</v>
+        <v>886</v>
       </c>
       <c r="B17" s="0">
-        <v>0.12509458329340301</v>
+        <v>0.20984326579628981</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>17</v>
+        <v>887</v>
       </c>
       <c r="B18" s="0">
-        <v>0.17677894600984828</v>
+        <v>0.30610623894668854</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>18</v>
+        <v>888</v>
       </c>
       <c r="B19" s="0">
-        <v>0.23017584753781614</v>
+        <v>0.37898262506760499</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>19</v>
+        <v>889</v>
       </c>
       <c r="B20" s="0">
-        <v>0.33659455720543618</v>
+        <v>0.51234475398656487</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>20</v>
+        <v>890</v>
       </c>
       <c r="B21" s="0">
-        <v>0.43224254881854196</v>
+        <v>0.6068549097414494</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>21</v>
+        <v>891</v>
       </c>
       <c r="B22" s="0">
-        <v>0.50092904724663556</v>
+        <v>0.66732965782208831</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>22</v>
+        <v>892</v>
       </c>
       <c r="B23" s="0">
-        <v>0.14126959819230683</v>
+        <v>0.26590518210338454</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>23</v>
+        <v>893</v>
       </c>
       <c r="B24" s="0">
-        <v>0.19212156077059375</v>
+        <v>0.34432915780252465</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>24</v>
+        <v>894</v>
       </c>
       <c r="B25" s="0">
-        <v>0.25400323508238681</v>
+        <v>0.43446819619628602</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>25</v>
+        <v>895</v>
       </c>
       <c r="B26" s="0">
-        <v>0.36657253201217987</v>
+        <v>0.56603903469722483</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>26</v>
+        <v>896</v>
       </c>
       <c r="B27" s="0">
-        <v>0.47094334222220174</v>
+        <v>0.66629544098097226</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>27</v>
+        <v>897</v>
       </c>
       <c r="B28" s="0">
-        <v>0.1814922808743028</v>
+        <v>0.31337209638160929</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>28</v>
+        <v>898</v>
       </c>
       <c r="B29" s="0">
-        <v>0.11660531077899448</v>
+        <v>0.22431324716624609</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>29</v>
+        <v>899</v>
       </c>
       <c r="B30" s="0">
-        <v>0.22641741468840526</v>
+        <v>0.56089893560369752</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>30</v>
+        <v>900</v>
       </c>
       <c r="B31" s="0">
-        <v>0.25426058160740872</v>
+        <v>0.62448781497805306</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>31</v>
+        <v>901</v>
       </c>
       <c r="B32" s="0">
-        <v>0.52200579408603676</v>
+        <v>0.75099762261481362</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>32</v>
+        <v>902</v>
       </c>
       <c r="B33" s="0">
-        <v>0.13376101742055357</v>
+        <v>0.29840260743348068</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>33</v>
+        <v>903</v>
       </c>
       <c r="B34" s="0">
-        <v>0.68756875546608875</v>
+        <v>0.83908528167365859</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>34</v>
+        <v>904</v>
       </c>
       <c r="B35" s="0"/>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>35</v>
+        <v>905</v>
       </c>
       <c r="B36" s="0">
-        <v>8.8635007362911153</v>
+        <v>11.104787872367531</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>36</v>
+        <v>906</v>
       </c>
       <c r="B37" s="0">
-        <v>7.3337981445657316</v>
+        <v>9.0036620304295649</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>37</v>
+        <v>907</v>
       </c>
       <c r="B38" s="0">
-        <v>23.958357281125171</v>
+        <v>26.937285645120284</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>38</v>
+        <v>908</v>
       </c>
       <c r="B39" s="0">
-        <v>22.705315546713319</v>
+        <v>24.99279642981546</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>39</v>
+        <v>909</v>
       </c>
       <c r="B40" s="0"/>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>40</v>
+        <v>910</v>
       </c>
       <c r="B41" s="0">
-        <v>16.123433593698834</v>
+        <v>20.30558270872065</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>41</v>
+        <v>911</v>
       </c>
       <c r="B42" s="0">
-        <v>16.123433593691615</v>
+        <v>20.305582708736136</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>42</v>
+        <v>912</v>
       </c>
       <c r="B43" s="0">
-        <v>22.823369447987879</v>
+        <v>34.602168932553326</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>43</v>
+        <v>913</v>
       </c>
       <c r="B44" s="0">
-        <v>33.789459893141924</v>
+        <v>38.261310376231251</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>44</v>
+        <v>914</v>
       </c>
       <c r="B45" s="0">
-        <v>33.789459893122185</v>
+        <v>38.261310376235031</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>45</v>
+        <v>915</v>
       </c>
       <c r="B46" s="0">
-        <v>37.53550013107629</v>
+        <v>47.285445583654059</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>46</v>
+        <v>916</v>
       </c>
       <c r="B47" s="0"/>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>47</v>
+        <v>917</v>
       </c>
       <c r="B48" s="0">
-        <v>25.984586043135309</v>
+        <v>23.886404708083838</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>48</v>
+        <v>918</v>
       </c>
       <c r="B49" s="0">
-        <v>18.932917325466157</v>
+        <v>26.048712289959973</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>49</v>
+        <v>919</v>
       </c>
       <c r="B50" s="0">
-        <v>28.131388062834944</v>
+        <v>21.053425205937806</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>50</v>
+        <v>920</v>
       </c>
       <c r="B51" s="0">
-        <v>49.116223246726577</v>
+        <v>43.883027738162795</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>51</v>
+        <v>921</v>
       </c>
       <c r="B52" s="0">
-        <v>37.603405131565871</v>
+        <v>44.112263026335199</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>52</v>
+        <v>922</v>
       </c>
       <c r="B53" s="0">
-        <v>52.621172524921114</v>
+        <v>43.582691709188879</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>53</v>
+        <v>923</v>
       </c>
       <c r="B54" s="0"/>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>54</v>
+        <v>924</v>
       </c>
       <c r="B55" s="0">
-        <v>0.0038008014254332354</v>
+        <v>0.0039355083526632483</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>55</v>
+        <v>925</v>
       </c>
       <c r="B56" s="0">
-        <v>0.035299712564309534</v>
+        <v>0.058143186836911845</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>56</v>
+        <v>926</v>
       </c>
       <c r="B57" s="0">
-        <v>0.24704698512579756</v>
+        <v>0.32301171297246056</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>57</v>
+        <v>927</v>
       </c>
       <c r="B58" s="0">
-        <v>2.7430929084387734</v>
+        <v>7.6666065942917188</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>58</v>
+        <v>928</v>
       </c>
       <c r="B59" s="0">
-        <v>4.0665296542262714</v>
+        <v>13.356409391587615</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>59</v>
+        <v>929</v>
       </c>
       <c r="B60" s="0">
-        <v>5.7946684521443776</v>
+        <v>49.619019456929152</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>60</v>
+        <v>930</v>
       </c>
       <c r="B61" s="0">
-        <v>7.9256764583645172</v>
+        <v>49.840460224913912</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>61</v>
+        <v>931</v>
       </c>
       <c r="B62" s="0">
-        <v>17.592461983405705</v>
+        <v>191.73474476403169</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>62</v>
+        <v>932</v>
       </c>
       <c r="B63" s="0"/>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>63</v>
+        <v>933</v>
       </c>
       <c r="B64" s="0">
-        <v>0.0016986998857169092</v>
+        <v>0.00010427131170060511</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>64</v>
+        <v>934</v>
       </c>
       <c r="B65" s="0">
-        <v>0.024257202694173682</v>
+        <v>0.0062025354041632995</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>65</v>
+        <v>935</v>
       </c>
       <c r="B66" s="0">
-        <v>0.15095320303095686</v>
+        <v>0.049999982106113131</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>66</v>
+        <v>936</v>
       </c>
       <c r="B67" s="0">
-        <v>1.4887931501324487</v>
+        <v>0.8745878080223749</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>67</v>
+        <v>937</v>
       </c>
       <c r="B68" s="0">
-        <v>2.3338937936705193</v>
+        <v>1.4844110403983231</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>68</v>
+        <v>938</v>
       </c>
       <c r="B69" s="0">
-        <v>3.5899561974658787</v>
+        <v>2.437153937842524</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>69</v>
+        <v>939</v>
       </c>
       <c r="B70" s="0">
-        <v>4.5806166118511635</v>
+        <v>3.2455353397225473</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>70</v>
+        <v>940</v>
       </c>
       <c r="B71" s="0">
-        <v>8.1397833160762918</v>
+        <v>6.7449538375700584</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>71</v>
+        <v>941</v>
       </c>
       <c r="B72" s="0"/>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>72</v>
+        <v>942</v>
       </c>
       <c r="B73" s="0">
         <v>0</v>
@@ -1070,7 +3692,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>73</v>
+        <v>943</v>
       </c>
       <c r="B74" s="0">
         <v>0</v>
@@ -1078,121 +3700,121 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>74</v>
+        <v>944</v>
       </c>
       <c r="B75" s="0">
-        <v>0</v>
+        <v>0.029076104242392289</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>75</v>
+        <v>945</v>
       </c>
       <c r="B76" s="0">
-        <v>0.12643790364053323</v>
+        <v>4.452263760407094</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>76</v>
+        <v>946</v>
       </c>
       <c r="B77" s="0">
-        <v>0.61341977952748927</v>
+        <v>10.481177866698536</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>77</v>
+        <v>947</v>
       </c>
       <c r="B78" s="0">
-        <v>1.5410472911681896</v>
+        <v>28.15380099628505</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>78</v>
+        <v>948</v>
       </c>
       <c r="B79" s="0">
-        <v>3.0663548424304619</v>
+        <v>47.753979399730454</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>79</v>
+        <v>949</v>
       </c>
       <c r="B80" s="0">
-        <v>11.266959258620405</v>
+        <v>169.75104472544584</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>80</v>
+        <v>950</v>
       </c>
       <c r="B81" s="0"/>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>81</v>
+        <v>951</v>
       </c>
       <c r="B82" s="0"/>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>82</v>
+        <v>952</v>
       </c>
       <c r="B83" s="0"/>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>83</v>
+        <v>953</v>
       </c>
       <c r="B84" s="0"/>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>84</v>
+        <v>954</v>
       </c>
       <c r="B85" s="0"/>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>85</v>
+        <v>955</v>
       </c>
       <c r="B86" s="0"/>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>86</v>
+        <v>956</v>
       </c>
       <c r="B87" s="0"/>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>87</v>
+        <v>957</v>
       </c>
       <c r="B88" s="0"/>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>88</v>
+        <v>958</v>
       </c>
       <c r="B89" s="0"/>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>89</v>
+        <v>959</v>
       </c>
       <c r="B90" s="0"/>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>90</v>
+        <v>960</v>
       </c>
       <c r="B91" s="0"/>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>91</v>
+        <v>961</v>
       </c>
       <c r="B92" s="0">
         <v>0</v>
@@ -1200,7 +3822,7 @@
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>92</v>
+        <v>962</v>
       </c>
       <c r="B93" s="0">
         <v>0.20000000000000001</v>
@@ -1208,109 +3830,109 @@
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>93</v>
+        <v>963</v>
       </c>
       <c r="B94" s="0">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>94</v>
+        <v>964</v>
       </c>
       <c r="B95" s="0">
-        <v>24.999999999999996</v>
+        <v>624.99999999999989</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>95</v>
+        <v>965</v>
       </c>
       <c r="B96" s="0">
-        <v>0.0063146461903739537</v>
+        <v>0.0074480424928103682</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>96</v>
+        <v>966</v>
       </c>
       <c r="B97" s="0">
-        <v>0.00021960860690324016</v>
+        <v>0.0026440155506744631</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>97</v>
+        <v>967</v>
       </c>
       <c r="B98" s="0">
-        <v>0.089118220119267191</v>
+        <v>0.112122124240448</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>98</v>
+        <v>968</v>
       </c>
       <c r="B99" s="0">
-        <v>0.048146936696367305</v>
+        <v>0.069330549340421294</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>99</v>
+        <v>969</v>
       </c>
       <c r="B100" s="0">
-        <v>0.0061173693442384477</v>
+        <v>0.014726898765277788</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>100</v>
+        <v>970</v>
       </c>
       <c r="B101" s="0">
-        <v>0.014744957143121983</v>
+        <v>0.040722864868775514</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>101</v>
+        <v>971</v>
       </c>
       <c r="B102" s="0">
-        <v>0.038775598712182148</v>
+        <v>0.055422565381061113</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>102</v>
+        <v>972</v>
       </c>
       <c r="B103" s="0">
-        <v>0.10398581470825477</v>
+        <v>0.13631708688875901</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>103</v>
+        <v>973</v>
       </c>
       <c r="B104" s="0">
-        <v>0.12381563054508873</v>
+        <v>0.16488212785474907</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>104</v>
+        <v>974</v>
       </c>
       <c r="B105" s="0">
-        <v>0.1757730297036168</v>
+        <v>0.21655691284224937</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>105</v>
+        <v>975</v>
       </c>
       <c r="B106" s="0"/>
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>106</v>
+        <v>976</v>
       </c>
       <c r="B107" s="0">
         <v>1</v>
@@ -1318,7 +3940,7 @@
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>107</v>
+        <v>977</v>
       </c>
       <c r="B108" s="0">
         <v>0.0025000000000000001</v>
@@ -1326,15 +3948,15 @@
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>108</v>
+        <v>978</v>
       </c>
       <c r="B109" s="0">
-        <v>0.0070000000000000001</v>
+        <v>0.012195554436469575</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>109</v>
+        <v>979</v>
       </c>
       <c r="B110" s="0">
         <v>0.0050000000000000001</v>
@@ -1342,7 +3964,7 @@
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>110</v>
+        <v>980</v>
       </c>
       <c r="B111" s="0" t="b">
         <v>0</v>
@@ -1350,7 +3972,7 @@
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>111</v>
+        <v>981</v>
       </c>
       <c r="B112" s="0">
         <v>20</v>
@@ -1358,7 +3980,7 @@
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>112</v>
+        <v>982</v>
       </c>
       <c r="B113" s="0">
         <v>500</v>
@@ -1366,7 +3988,7 @@
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>113</v>
+        <v>983</v>
       </c>
       <c r="B114" s="0">
         <v>0</v>
@@ -1374,7 +3996,7 @@
     </row>
     <row r="115">
       <c r="A115" s="0" t="s">
-        <v>114</v>
+        <v>984</v>
       </c>
       <c r="B115" s="0">
         <v>1</v>
@@ -1382,216 +4004,216 @@
     </row>
     <row r="116">
       <c r="A116" s="0" t="s">
-        <v>115</v>
+        <v>985</v>
       </c>
       <c r="B116" s="0">
-        <v>79181</v>
+        <v>67131.732999999993</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="s">
-        <v>116</v>
+        <v>986</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>144</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="s">
-        <v>117</v>
+        <v>987</v>
       </c>
       <c r="B118" s="0"/>
     </row>
     <row r="119">
       <c r="A119" s="0" t="s">
-        <v>118</v>
+        <v>988</v>
       </c>
       <c r="B119" s="0">
-        <v>0.60215040035305001</v>
+        <v>0.34343538750277502</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="s">
-        <v>119</v>
+        <v>989</v>
       </c>
       <c r="B120" s="0">
-        <v>0.61539541355313809</v>
+        <v>0.35740211980521641</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="s">
-        <v>120</v>
+        <v>990</v>
       </c>
       <c r="B121" s="0">
-        <v>0.62923352630368379</v>
+        <v>0.37195131295429584</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="s">
-        <v>121</v>
+        <v>991</v>
       </c>
       <c r="B122" s="0">
-        <v>0.65832112965162115</v>
+        <v>0.40243331636118962</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="s">
-        <v>122</v>
+        <v>992</v>
       </c>
       <c r="B123" s="0">
-        <v>0.75025238798872018</v>
+        <v>0.49840048569052708</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="s">
-        <v>123</v>
+        <v>993</v>
       </c>
       <c r="B124" s="0">
-        <v>0.87488214965163413</v>
+        <v>0.62976444652678509</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="s">
-        <v>124</v>
+        <v>994</v>
       </c>
       <c r="B125" s="0">
-        <v>0.61898013946723662</v>
+        <v>0.36445839428153387</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="s">
-        <v>125</v>
+        <v>995</v>
       </c>
       <c r="B126" s="0">
-        <v>0.6367172928900855</v>
+        <v>0.38667504345179493</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="s">
-        <v>126</v>
+        <v>996</v>
       </c>
       <c r="B127" s="0">
-        <v>0.67417271777093402</v>
+        <v>0.43348689974787014</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="s">
-        <v>127</v>
+        <v>997</v>
       </c>
       <c r="B128" s="0">
-        <v>0.78904768865963915</v>
+        <v>0.57130828633936148</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="s">
-        <v>128</v>
+        <v>998</v>
       </c>
       <c r="B129" s="0">
-        <v>0.89993330739435962</v>
+        <v>0.66583661539013672</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="s">
-        <v>129</v>
+        <v>999</v>
       </c>
       <c r="B130" s="0">
-        <v>0.052649334601238225</v>
+        <v>0.037829099640095613</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="s">
-        <v>130</v>
+        <v>1000</v>
       </c>
       <c r="B131" s="0">
-        <v>0.10132296293154838</v>
+        <v>0.098893880570689319</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="s">
-        <v>131</v>
+        <v>1001</v>
       </c>
       <c r="B132" s="0">
-        <v>0.13971350718757311</v>
+        <v>0.14409683132621545</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="s">
-        <v>132</v>
+        <v>1002</v>
       </c>
       <c r="B133" s="0">
-        <v>0.18136366360800679</v>
+        <v>0.1786826426564268</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="s">
-        <v>133</v>
+        <v>1003</v>
       </c>
       <c r="B134" s="0">
-        <v>0.27219083947834088</v>
+        <v>0.24387834263263777</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="s">
-        <v>134</v>
+        <v>1004</v>
       </c>
       <c r="B135" s="0">
-        <v>0.30602391302094689</v>
+        <v>0.27438040973226058</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="s">
-        <v>135</v>
+        <v>1005</v>
       </c>
       <c r="B136" s="0">
-        <v>0.11330263059960072</v>
+        <v>0.12521749133155899</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="s">
-        <v>136</v>
+        <v>1006</v>
       </c>
       <c r="B137" s="0">
-        <v>0.1513411370962528</v>
+        <v>0.1621339595153124</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="s">
-        <v>137</v>
+        <v>1007</v>
       </c>
       <c r="B138" s="0">
-        <v>0.2010405556866442</v>
+        <v>0.20560028402232194</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="s">
-        <v>138</v>
+        <v>1008</v>
       </c>
       <c r="B139" s="0">
-        <v>0.29410291894044538</v>
+        <v>0.26695641963424022</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="s">
-        <v>139</v>
+        <v>1009</v>
       </c>
       <c r="B140" s="0">
-        <v>0.30893381257174585</v>
+        <v>0.35044174419056917</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="s">
-        <v>140</v>
+        <v>1010</v>
       </c>
       <c r="B141" s="0">
-        <v>0.14039926785284126</v>
+        <v>0.13760202107326533</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="s">
-        <v>141</v>
+        <v>1011</v>
       </c>
       <c r="B142" s="0">
-        <v>0.086957176641814696</v>
+        <v>0.084232357572765121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lots of updates, now going to try to run menu cost on server using rho and rb to calibrate
</commit_message>
<xml_diff>
--- a/output/run1_table.xlsx
+++ b/output/run1_table.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2175" uniqueCount="2175">
   <si>
     <t>Row</t>
   </si>
@@ -3055,6 +3055,3486 @@
   </si>
   <si>
     <t>iy=1, kappa2=0.25</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>unnamed</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>unnamed</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>unnamed</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>unnamed</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>unnamed</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>unnamed</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>unnamed</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>unnamed</t>
   </si>
   <si>
     <t>cont_a, no meas err</t>
@@ -3078,7 +6558,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -3093,11 +6573,19 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -3106,6 +6594,14 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3124,53 +6620,53 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>870</v>
+        <v>2030</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1012</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>871</v>
+        <v>2031</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1013</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>872</v>
+        <v>2032</v>
       </c>
       <c r="B3" s="0">
-        <v>11.10478787236034</v>
+        <v>23.491115363196393</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>873</v>
+        <v>2033</v>
       </c>
       <c r="B4" s="0">
-        <v>26.937285645146559</v>
+        <v>35.638323103896397</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>874</v>
+        <v>2034</v>
       </c>
       <c r="B5" s="0">
-        <v>0.96932819366254985</v>
+        <v>0.99404007774605707</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>875</v>
+        <v>2035</v>
       </c>
       <c r="B6" s="0"/>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>876</v>
+        <v>2036</v>
       </c>
       <c r="B7" s="0">
         <v>1.0991047620773315</v>
@@ -3178,7 +6674,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>877</v>
+        <v>2037</v>
       </c>
       <c r="B8" s="0">
         <v>0.803355872631073</v>
@@ -3186,7 +6682,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>878</v>
+        <v>2038</v>
       </c>
       <c r="B9" s="0">
         <v>0.803355872631073</v>
@@ -3194,497 +6690,497 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>879</v>
+        <v>2039</v>
       </c>
       <c r="B10" s="0"/>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>880</v>
+        <v>2040</v>
       </c>
       <c r="B11" s="0">
-        <v>4.1000312263037682</v>
+        <v>4.1928734527103311</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>881</v>
+        <v>2041</v>
       </c>
       <c r="B12" s="0">
-        <v>0.41403322321604691</v>
+        <v>0.55977330595568153</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>882</v>
+        <v>2042</v>
       </c>
       <c r="B13" s="0">
-        <v>0.32301171297246056</v>
+        <v>1.3148822868167553</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>883</v>
+        <v>2043</v>
       </c>
       <c r="B14" s="0">
-        <v>0.049999982106113131</v>
+        <v>0.049881959099853032</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>884</v>
+        <v>2044</v>
       </c>
       <c r="B15" s="0">
-        <v>0.17916849052428613</v>
+        <v>0.43619287217730685</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>885</v>
+        <v>2045</v>
       </c>
       <c r="B16" s="0">
-        <v>0.079788190309264595</v>
+        <v>0.31551423125927114</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>886</v>
+        <v>2046</v>
       </c>
       <c r="B17" s="0">
-        <v>0.20984326579628981</v>
+        <v>0.36322784184673984</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>887</v>
+        <v>2047</v>
       </c>
       <c r="B18" s="0">
-        <v>0.30610623894668854</v>
+        <v>0.40022962008454405</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>888</v>
+        <v>2048</v>
       </c>
       <c r="B19" s="0">
-        <v>0.37898262506760499</v>
+        <v>0.43609665819805571</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>889</v>
+        <v>2049</v>
       </c>
       <c r="B20" s="0">
-        <v>0.51234475398656487</v>
+        <v>0.50548179593254716</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>890</v>
+        <v>2050</v>
       </c>
       <c r="B21" s="0">
-        <v>0.6068549097414494</v>
+        <v>0.56950795919495689</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>891</v>
+        <v>2051</v>
       </c>
       <c r="B22" s="0">
-        <v>0.66732965782208831</v>
+        <v>0.61739468638517581</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>892</v>
+        <v>2052</v>
       </c>
       <c r="B23" s="0">
-        <v>0.26590518210338454</v>
+        <v>0.3841151101612722</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>893</v>
+        <v>2053</v>
       </c>
       <c r="B24" s="0">
-        <v>0.34432915780252465</v>
+        <v>0.41889574901037813</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>894</v>
+        <v>2054</v>
       </c>
       <c r="B25" s="0">
-        <v>0.43446819619628602</v>
+        <v>0.4640613999463914</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>895</v>
+        <v>2055</v>
       </c>
       <c r="B26" s="0">
-        <v>0.56603903469722483</v>
+        <v>0.53926369710123723</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>896</v>
+        <v>2056</v>
       </c>
       <c r="B27" s="0">
-        <v>0.66629544098097226</v>
+        <v>0.61653246543405593</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>897</v>
+        <v>2057</v>
       </c>
       <c r="B28" s="0">
-        <v>0.31337209638160929</v>
+        <v>0.39536042880682626</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>898</v>
+        <v>2058</v>
       </c>
       <c r="B29" s="0">
-        <v>0.22431324716624609</v>
+        <v>0.35962985066288056</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>899</v>
+        <v>2059</v>
       </c>
       <c r="B30" s="0">
-        <v>0.56089893560369752</v>
+        <v>0.81594201550490419</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>900</v>
+        <v>2060</v>
       </c>
       <c r="B31" s="0">
-        <v>0.62448781497805306</v>
+        <v>0.8758385107787694</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>901</v>
+        <v>2061</v>
       </c>
       <c r="B32" s="0">
-        <v>0.75099762261481362</v>
+        <v>0.36385370385249216</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>902</v>
+        <v>2062</v>
       </c>
       <c r="B33" s="0">
-        <v>0.29840260743348068</v>
+        <v>0.067974650722921193</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>903</v>
+        <v>2063</v>
       </c>
       <c r="B34" s="0">
-        <v>0.83908528167365859</v>
+        <v>0.62945652838885069</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>904</v>
+        <v>2064</v>
       </c>
       <c r="B35" s="0"/>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>905</v>
+        <v>2065</v>
       </c>
       <c r="B36" s="0">
-        <v>11.104787872367531</v>
+        <v>23.49111536318572</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>906</v>
+        <v>2066</v>
       </c>
       <c r="B37" s="0">
-        <v>9.0036620304295649</v>
+        <v>15.148070929356896</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>907</v>
+        <v>2067</v>
       </c>
       <c r="B38" s="0">
-        <v>26.937285645120284</v>
+        <v>35.638323103879017</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>908</v>
+        <v>2068</v>
       </c>
       <c r="B39" s="0">
-        <v>24.99279642981546</v>
+        <v>30.627215709450724</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>909</v>
+        <v>2069</v>
       </c>
       <c r="B40" s="0"/>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>910</v>
+        <v>2070</v>
       </c>
       <c r="B41" s="0">
-        <v>20.30558270872065</v>
+        <v>37.485549168552232</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>911</v>
+        <v>2071</v>
       </c>
       <c r="B42" s="0">
-        <v>20.305582708736136</v>
+        <v>37.485549168569761</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>912</v>
+        <v>2072</v>
       </c>
       <c r="B43" s="0">
-        <v>34.602168932553326</v>
+        <v>43.118890253481645</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>913</v>
+        <v>2073</v>
       </c>
       <c r="B44" s="0">
-        <v>38.261310376231251</v>
+        <v>47.93734101898167</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>914</v>
+        <v>2074</v>
       </c>
       <c r="B45" s="0">
-        <v>38.261310376235031</v>
+        <v>47.937341018982735</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>915</v>
+        <v>2075</v>
       </c>
       <c r="B46" s="0">
-        <v>47.285445583654059</v>
+        <v>51.574352331412143</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>916</v>
+        <v>2076</v>
       </c>
       <c r="B47" s="0"/>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>917</v>
+        <v>2077</v>
       </c>
       <c r="B48" s="0">
-        <v>23.886404708083838</v>
+        <v>54.70344428733074</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>918</v>
+        <v>2078</v>
       </c>
       <c r="B49" s="0">
-        <v>26.048712289959973</v>
+        <v>60.963440288481998</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>919</v>
+        <v>2079</v>
       </c>
       <c r="B50" s="0">
-        <v>21.053425205937806</v>
+        <v>24.365066974450141</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>920</v>
+        <v>2080</v>
       </c>
       <c r="B51" s="0">
-        <v>43.883027738162795</v>
+        <v>70.888802939876925</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>921</v>
+        <v>2081</v>
       </c>
       <c r="B52" s="0">
-        <v>44.112263026335199</v>
+        <v>75.651459648385796</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>922</v>
+        <v>2082</v>
       </c>
       <c r="B53" s="0">
-        <v>43.582691709188879</v>
+        <v>47.807114675556761</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>923</v>
+        <v>2083</v>
       </c>
       <c r="B54" s="0"/>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>924</v>
+        <v>2084</v>
       </c>
       <c r="B55" s="0">
-        <v>0.0039355083526632483</v>
+        <v>0.013200717753390783</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>925</v>
+        <v>2085</v>
       </c>
       <c r="B56" s="0">
-        <v>0.058143186836911845</v>
+        <v>0.22404653438592209</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>926</v>
+        <v>2086</v>
       </c>
       <c r="B57" s="0">
-        <v>0.32301171297246056</v>
+        <v>1.3148822868167553</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>927</v>
+        <v>2087</v>
       </c>
       <c r="B58" s="0">
-        <v>7.6666065942917188</v>
+        <v>12.786555498378227</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>928</v>
+        <v>2088</v>
       </c>
       <c r="B59" s="0">
-        <v>13.356409391587615</v>
+        <v>12.83535746989258</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>929</v>
+        <v>2089</v>
       </c>
       <c r="B60" s="0">
-        <v>49.619019456929152</v>
+        <v>15.054940606516276</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>930</v>
+        <v>2090</v>
       </c>
       <c r="B61" s="0">
-        <v>49.840460224913912</v>
+        <v>26.270145372069717</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>931</v>
+        <v>2091</v>
       </c>
       <c r="B62" s="0">
-        <v>191.73474476403169</v>
+        <v>30.059369242172899</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>932</v>
+        <v>2092</v>
       </c>
       <c r="B63" s="0"/>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>933</v>
+        <v>2093</v>
       </c>
       <c r="B64" s="0">
-        <v>0.00010427131170060511</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>934</v>
+        <v>2094</v>
       </c>
       <c r="B65" s="0">
-        <v>0.0062025354041632995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>935</v>
+        <v>2095</v>
       </c>
       <c r="B66" s="0">
-        <v>0.049999982106113131</v>
+        <v>0.049881959099853032</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>936</v>
+        <v>2096</v>
       </c>
       <c r="B67" s="0">
-        <v>0.8745878080223749</v>
+        <v>1.168088384065751</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>937</v>
+        <v>2097</v>
       </c>
       <c r="B68" s="0">
-        <v>1.4844110403983231</v>
+        <v>1.9791726905717764</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>938</v>
+        <v>2098</v>
       </c>
       <c r="B69" s="0">
-        <v>2.437153937842524</v>
+        <v>3.7582008717874227</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>939</v>
+        <v>2099</v>
       </c>
       <c r="B70" s="0">
-        <v>3.2455353397225473</v>
+        <v>5.1382638184815619</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>940</v>
+        <v>2100</v>
       </c>
       <c r="B71" s="0">
-        <v>6.7449538375700584</v>
+        <v>10.210418515428744</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>941</v>
+        <v>2101</v>
       </c>
       <c r="B72" s="0"/>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>942</v>
+        <v>2102</v>
       </c>
       <c r="B73" s="0">
         <v>0</v>
@@ -3692,7 +7188,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>943</v>
+        <v>2103</v>
       </c>
       <c r="B74" s="0">
         <v>0</v>
@@ -3700,153 +7196,153 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>944</v>
+        <v>2104</v>
       </c>
       <c r="B75" s="0">
-        <v>0.029076104242392289</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>945</v>
+        <v>2105</v>
       </c>
       <c r="B76" s="0">
-        <v>4.452263760407094</v>
+        <v>6.5024545032956524</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>946</v>
+        <v>2106</v>
       </c>
       <c r="B77" s="0">
-        <v>10.481177866698536</v>
+        <v>8.9931608450129659</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>947</v>
+        <v>2107</v>
       </c>
       <c r="B78" s="0">
-        <v>28.15380099628505</v>
+        <v>11.812413233991226</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>948</v>
+        <v>2108</v>
       </c>
       <c r="B79" s="0">
-        <v>47.753979399730454</v>
+        <v>13.06335406459238</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>949</v>
+        <v>2109</v>
       </c>
       <c r="B80" s="0">
-        <v>169.75104472544584</v>
+        <v>24.44451824650675</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>950</v>
+        <v>2110</v>
       </c>
       <c r="B81" s="0"/>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>951</v>
+        <v>2111</v>
       </c>
       <c r="B82" s="0"/>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>952</v>
+        <v>2112</v>
       </c>
       <c r="B83" s="0"/>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>953</v>
+        <v>2113</v>
       </c>
       <c r="B84" s="0"/>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>954</v>
+        <v>2114</v>
       </c>
       <c r="B85" s="0"/>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>955</v>
+        <v>2115</v>
       </c>
       <c r="B86" s="0"/>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>956</v>
+        <v>2116</v>
       </c>
       <c r="B87" s="0"/>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>957</v>
+        <v>2117</v>
       </c>
       <c r="B88" s="0"/>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>958</v>
+        <v>2118</v>
       </c>
       <c r="B89" s="0"/>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>959</v>
+        <v>2119</v>
       </c>
       <c r="B90" s="0"/>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>960</v>
+        <v>2120</v>
       </c>
       <c r="B91" s="0"/>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>961</v>
+        <v>2121</v>
       </c>
       <c r="B92" s="0">
-        <v>0</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>962</v>
+        <v>2122</v>
       </c>
       <c r="B93" s="0">
-        <v>0.20000000000000001</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>963</v>
+        <v>2123</v>
       </c>
       <c r="B94" s="0">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>964</v>
+        <v>2124</v>
       </c>
       <c r="B95" s="0">
-        <v>624.99999999999989</v>
+        <v>9.9999999999999998e-13</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>965</v>
+        <v>2125</v>
       </c>
       <c r="B96" s="0">
         <v>0.0074480424928103682</v>
@@ -3854,109 +7350,95 @@
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>966</v>
+        <v>2126</v>
       </c>
       <c r="B97" s="0">
-        <v>0.0026440155506744631</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>967</v>
+        <v>2127</v>
       </c>
       <c r="B98" s="0">
-        <v>0.112122124240448</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>968</v>
+        <v>2128</v>
       </c>
       <c r="B99" s="0">
-        <v>0.069330549340421294</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>969</v>
-      </c>
-      <c r="B100" s="0">
-        <v>0.014726898765277788</v>
-      </c>
+        <v>2129</v>
+      </c>
+      <c r="B100" s="0"/>
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>970</v>
-      </c>
-      <c r="B101" s="0">
-        <v>0.040722864868775514</v>
-      </c>
+        <v>2130</v>
+      </c>
+      <c r="B101" s="0"/>
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>971</v>
-      </c>
-      <c r="B102" s="0">
-        <v>0.055422565381061113</v>
-      </c>
+        <v>2131</v>
+      </c>
+      <c r="B102" s="0"/>
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>972</v>
-      </c>
-      <c r="B103" s="0">
-        <v>0.13631708688875901</v>
-      </c>
+        <v>2132</v>
+      </c>
+      <c r="B103" s="0"/>
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>973</v>
-      </c>
-      <c r="B104" s="0">
-        <v>0.16488212785474907</v>
-      </c>
+        <v>2133</v>
+      </c>
+      <c r="B104" s="0"/>
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>974</v>
-      </c>
-      <c r="B105" s="0">
-        <v>0.21655691284224937</v>
-      </c>
+        <v>2134</v>
+      </c>
+      <c r="B105" s="0"/>
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>975</v>
+        <v>2135</v>
       </c>
       <c r="B106" s="0"/>
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>976</v>
-      </c>
-      <c r="B107" s="0">
-        <v>1</v>
-      </c>
+        <v>2136</v>
+      </c>
+      <c r="B107" s="0"/>
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>977</v>
+        <v>2137</v>
       </c>
       <c r="B108" s="0">
-        <v>0.0025000000000000001</v>
+        <v>0.0020773236596895272</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>978</v>
+        <v>2138</v>
       </c>
       <c r="B109" s="0">
-        <v>0.012195554436469575</v>
+        <v>0.0030000000000000001</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>979</v>
+        <v>2139</v>
       </c>
       <c r="B110" s="0">
         <v>0.0050000000000000001</v>
@@ -3964,7 +7446,7 @@
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>980</v>
+        <v>2140</v>
       </c>
       <c r="B111" s="0" t="b">
         <v>0</v>
@@ -3972,7 +7454,7 @@
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>981</v>
+        <v>2141</v>
       </c>
       <c r="B112" s="0">
         <v>20</v>
@@ -3980,7 +7462,7 @@
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>982</v>
+        <v>2142</v>
       </c>
       <c r="B113" s="0">
         <v>500</v>
@@ -3988,7 +7470,7 @@
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>983</v>
+        <v>2143</v>
       </c>
       <c r="B114" s="0">
         <v>0</v>
@@ -3996,7 +7478,7 @@
     </row>
     <row r="115">
       <c r="A115" s="0" t="s">
-        <v>984</v>
+        <v>2144</v>
       </c>
       <c r="B115" s="0">
         <v>1</v>
@@ -4004,7 +7486,7 @@
     </row>
     <row r="116">
       <c r="A116" s="0" t="s">
-        <v>985</v>
+        <v>2145</v>
       </c>
       <c r="B116" s="0">
         <v>67131.732999999993</v>
@@ -4012,208 +7494,208 @@
     </row>
     <row r="117">
       <c r="A117" s="0" t="s">
-        <v>986</v>
+        <v>2146</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>1014</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="s">
-        <v>987</v>
+        <v>2147</v>
       </c>
       <c r="B118" s="0"/>
     </row>
     <row r="119">
       <c r="A119" s="0" t="s">
-        <v>988</v>
+        <v>2148</v>
       </c>
       <c r="B119" s="0">
-        <v>0.34343538750277502</v>
+        <v>0.51223045202004069</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="s">
-        <v>989</v>
+        <v>2149</v>
       </c>
       <c r="B120" s="0">
-        <v>0.35740211980521641</v>
+        <v>0.51328421275968772</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="s">
-        <v>990</v>
+        <v>2150</v>
       </c>
       <c r="B121" s="0">
-        <v>0.37195131295429584</v>
+        <v>0.51436406958828651</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="s">
-        <v>991</v>
+        <v>2151</v>
       </c>
       <c r="B122" s="0">
-        <v>0.40243331636118962</v>
+        <v>0.51658487145535148</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="s">
-        <v>992</v>
+        <v>2152</v>
       </c>
       <c r="B123" s="0">
-        <v>0.49840048569052708</v>
+        <v>0.52342638170970945</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="s">
-        <v>993</v>
+        <v>2153</v>
       </c>
       <c r="B124" s="0">
-        <v>0.62976444652678509</v>
+        <v>0.53336190747233603</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="s">
-        <v>994</v>
+        <v>2154</v>
       </c>
       <c r="B125" s="0">
-        <v>0.36445839428153387</v>
+        <v>0.51380992601184727</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="s">
-        <v>995</v>
+        <v>2155</v>
       </c>
       <c r="B126" s="0">
-        <v>0.38667504345179493</v>
+        <v>0.51544263391625855</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="s">
-        <v>996</v>
+        <v>2156</v>
       </c>
       <c r="B127" s="0">
-        <v>0.43348689974787014</v>
+        <v>0.51881089938924119</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="s">
-        <v>997</v>
+        <v>2157</v>
       </c>
       <c r="B128" s="0">
-        <v>0.57130828633936148</v>
+        <v>0.52871515579569972</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="s">
-        <v>998</v>
+        <v>2158</v>
       </c>
       <c r="B129" s="0">
-        <v>0.66583661539013672</v>
+        <v>0.53855530675886076</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="s">
-        <v>999</v>
+        <v>2159</v>
       </c>
       <c r="B130" s="0">
-        <v>0.037829099640095613</v>
+        <v>0.024207624860011785</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="s">
-        <v>1000</v>
+        <v>2160</v>
       </c>
       <c r="B131" s="0">
-        <v>0.098893880570689319</v>
+        <v>0.058151029926492181</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="s">
-        <v>1001</v>
+        <v>2161</v>
       </c>
       <c r="B132" s="0">
-        <v>0.14409683132621545</v>
+        <v>0.085156268608744534</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="s">
-        <v>1002</v>
+        <v>2162</v>
       </c>
       <c r="B133" s="0">
-        <v>0.1786826426564268</v>
+        <v>0.11573036985589466</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="s">
-        <v>1003</v>
+        <v>2163</v>
       </c>
       <c r="B134" s="0">
-        <v>0.24387834263263777</v>
+        <v>0.1842080455542438</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="s">
-        <v>1004</v>
+        <v>2164</v>
       </c>
       <c r="B135" s="0">
-        <v>0.27438040973226058</v>
+        <v>0.20696699758572265</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="s">
-        <v>1005</v>
+        <v>2165</v>
       </c>
       <c r="B136" s="0">
-        <v>0.12521749133155899</v>
+        <v>0.073144349889313162</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="s">
-        <v>1006</v>
+        <v>2166</v>
       </c>
       <c r="B137" s="0">
-        <v>0.1621339595153124</v>
+        <v>0.10060340058433585</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="s">
-        <v>1007</v>
+        <v>2167</v>
       </c>
       <c r="B138" s="0">
-        <v>0.20560028402232194</v>
+        <v>0.14220275134473714</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="s">
-        <v>1008</v>
+        <v>2168</v>
       </c>
       <c r="B139" s="0">
-        <v>0.26695641963424022</v>
+        <v>0.20663110085553599</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="s">
-        <v>1009</v>
+        <v>2169</v>
       </c>
       <c r="B140" s="0">
-        <v>0.35044174419056917</v>
+        <v>0.20780686716031577</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="s">
-        <v>1010</v>
+        <v>2170</v>
       </c>
       <c r="B141" s="0">
-        <v>0.13760202107326533</v>
+        <v>0.072769243675301243</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="s">
-        <v>1011</v>
+        <v>2171</v>
       </c>
       <c r="B142" s="0">
-        <v>0.084232357572765121</v>
+        <v>0.044652177826712006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected some menu cost stuff, now ready to retry batch
</commit_message>
<xml_diff>
--- a/output/run1_table.xlsx
+++ b/output/run1_table.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2175" uniqueCount="2175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2320" uniqueCount="2320">
   <si>
     <t>Row</t>
   </si>
@@ -6535,6 +6535,441 @@
   </si>
   <si>
     <t>unnamed</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>cal=1, r_a=2.000000e-02, reb_cost=1.489608e-03</t>
   </si>
   <si>
     <t>cont_a, no meas err</t>
@@ -6558,7 +6993,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -6581,11 +7016,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -6602,6 +7038,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6615,58 +7052,58 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="69.42578125" customWidth="true"/>
-    <col min="2" max="2" width="18.42578125" customWidth="true"/>
+    <col min="2" max="2" width="42.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>2030</v>
+        <v>2175</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>2172</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>2031</v>
+        <v>2176</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2173</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2032</v>
+        <v>2177</v>
       </c>
       <c r="B3" s="0">
-        <v>23.491115363196393</v>
+        <v>16.797546998531971</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>2033</v>
+        <v>2178</v>
       </c>
       <c r="B4" s="0">
-        <v>35.638323103896397</v>
+        <v>40.643693986181724</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>2034</v>
+        <v>2179</v>
       </c>
       <c r="B5" s="0">
-        <v>0.99404007774605707</v>
+        <v>0.92101277298502415</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>2035</v>
+        <v>2180</v>
       </c>
       <c r="B6" s="0"/>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>2036</v>
+        <v>2181</v>
       </c>
       <c r="B7" s="0">
         <v>1.0991047620773315</v>
@@ -6674,7 +7111,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>2037</v>
+        <v>2182</v>
       </c>
       <c r="B8" s="0">
         <v>0.803355872631073</v>
@@ -6682,7 +7119,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>2038</v>
+        <v>2183</v>
       </c>
       <c r="B9" s="0">
         <v>0.803355872631073</v>
@@ -6690,427 +7127,427 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>2039</v>
+        <v>2184</v>
       </c>
       <c r="B10" s="0"/>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>2040</v>
+        <v>2185</v>
       </c>
       <c r="B11" s="0">
-        <v>4.1928734527103311</v>
+        <v>4.0795939386802811</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>2041</v>
+        <v>2186</v>
       </c>
       <c r="B12" s="0">
-        <v>0.55977330595568153</v>
+        <v>0.56232947350128126</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>2042</v>
+        <v>2187</v>
       </c>
       <c r="B13" s="0">
-        <v>1.3148822868167553</v>
+        <v>0.1399000592045655</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>2043</v>
+        <v>2188</v>
       </c>
       <c r="B14" s="0">
-        <v>0.049881959099853032</v>
+        <v>0.012662848290688854</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>2044</v>
+        <v>2189</v>
       </c>
       <c r="B15" s="0">
-        <v>0.43619287217730685</v>
+        <v>0.40756267474146241</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>2045</v>
+        <v>2190</v>
       </c>
       <c r="B16" s="0">
-        <v>0.31551423125927114</v>
+        <v>0.16792334799990671</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>2046</v>
+        <v>2191</v>
       </c>
       <c r="B17" s="0">
-        <v>0.36322784184673984</v>
+        <v>0.35031682300309164</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>2047</v>
+        <v>2192</v>
       </c>
       <c r="B18" s="0">
-        <v>0.40022962008454405</v>
+        <v>0.47655635851259415</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>2048</v>
+        <v>2193</v>
       </c>
       <c r="B19" s="0">
-        <v>0.43609665819805571</v>
+        <v>0.53011351634723081</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>2049</v>
+        <v>2194</v>
       </c>
       <c r="B20" s="0">
-        <v>0.50548179593254716</v>
+        <v>0.61591168817242936</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>2050</v>
+        <v>2195</v>
       </c>
       <c r="B21" s="0">
-        <v>0.56950795919495689</v>
+        <v>0.67664470488462414</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>2051</v>
+        <v>2196</v>
       </c>
       <c r="B22" s="0">
-        <v>0.61739468638517581</v>
+        <v>0.7209766708036689</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>2052</v>
+        <v>2197</v>
       </c>
       <c r="B23" s="0">
-        <v>0.3841151101612722</v>
+        <v>0.42735848809702609</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>2053</v>
+        <v>2198</v>
       </c>
       <c r="B24" s="0">
-        <v>0.41889574901037813</v>
+        <v>0.50542783834144667</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>2054</v>
+        <v>2199</v>
       </c>
       <c r="B25" s="0">
-        <v>0.4640613999463914</v>
+        <v>0.56790660062105836</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>2055</v>
+        <v>2200</v>
       </c>
       <c r="B26" s="0">
-        <v>0.53926369710123723</v>
+        <v>0.64733699141370571</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>2056</v>
+        <v>2201</v>
       </c>
       <c r="B27" s="0">
-        <v>0.61653246543405593</v>
+        <v>0.72020753546714633</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>2057</v>
+        <v>2202</v>
       </c>
       <c r="B28" s="0">
-        <v>0.39536042880682626</v>
+        <v>0.50411046679164873</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>2058</v>
+        <v>2203</v>
       </c>
       <c r="B29" s="0">
-        <v>0.35962985066288056</v>
+        <v>0.40225260986085187</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>2059</v>
+        <v>2204</v>
       </c>
       <c r="B30" s="0">
-        <v>0.81594201550490419</v>
+        <v>0.44181169180447877</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>2060</v>
+        <v>2205</v>
       </c>
       <c r="B31" s="0">
-        <v>0.8758385107787694</v>
+        <v>0.46686687028647222</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>2061</v>
+        <v>2206</v>
       </c>
       <c r="B32" s="0">
-        <v>0.36385370385249216</v>
+        <v>0.86258896035485622</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>2062</v>
+        <v>2207</v>
       </c>
       <c r="B33" s="0">
-        <v>0.067974650722921193</v>
+        <v>0.57925496632296536</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>2063</v>
+        <v>2208</v>
       </c>
       <c r="B34" s="0">
-        <v>0.62945652838885069</v>
+        <v>0.911983421591268</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>2064</v>
+        <v>2209</v>
       </c>
       <c r="B35" s="0"/>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>2065</v>
+        <v>2210</v>
       </c>
       <c r="B36" s="0">
-        <v>23.49111536318572</v>
+        <v>16.797546998525991</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>2066</v>
+        <v>2211</v>
       </c>
       <c r="B37" s="0">
-        <v>15.148070929356896</v>
+        <v>13.997199629235729</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>2067</v>
+        <v>2212</v>
       </c>
       <c r="B38" s="0">
-        <v>35.638323103879017</v>
+        <v>40.643693986158461</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>2068</v>
+        <v>2213</v>
       </c>
       <c r="B39" s="0">
-        <v>30.627215709450724</v>
+        <v>38.643388845311911</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>2069</v>
+        <v>2214</v>
       </c>
       <c r="B40" s="0"/>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>2070</v>
+        <v>2215</v>
       </c>
       <c r="B41" s="0">
-        <v>37.485549168552232</v>
+        <v>32.82006623527198</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>2071</v>
+        <v>2216</v>
       </c>
       <c r="B42" s="0">
-        <v>37.485549168569761</v>
+        <v>32.820066235285459</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>2072</v>
+        <v>2217</v>
       </c>
       <c r="B43" s="0">
-        <v>43.118890253481645</v>
+        <v>51.588456603163671</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>2073</v>
+        <v>2218</v>
       </c>
       <c r="B44" s="0">
-        <v>47.93734101898167</v>
+        <v>55.500440622710258</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>2074</v>
+        <v>2219</v>
       </c>
       <c r="B45" s="0">
-        <v>47.937341018982735</v>
+        <v>55.500440622698846</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>2075</v>
+        <v>2220</v>
       </c>
       <c r="B46" s="0">
-        <v>51.574352331412143</v>
+        <v>64.802849277509267</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>2076</v>
+        <v>2221</v>
       </c>
       <c r="B47" s="0"/>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>2077</v>
+        <v>2222</v>
       </c>
       <c r="B48" s="0">
-        <v>54.70344428733074</v>
+        <v>25.01515089267567</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>2078</v>
+        <v>2223</v>
       </c>
       <c r="B49" s="0">
-        <v>60.963440288481998</v>
+        <v>29.491861358078737</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>2079</v>
+        <v>2224</v>
       </c>
       <c r="B50" s="0">
-        <v>24.365066974450141</v>
+        <v>21.545251360383219</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>2080</v>
+        <v>2225</v>
       </c>
       <c r="B51" s="0">
-        <v>70.888802939876925</v>
+        <v>52.76044283642689</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>2081</v>
+        <v>2226</v>
       </c>
       <c r="B52" s="0">
-        <v>75.651459648385796</v>
+        <v>55.386493689334657</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>2082</v>
+        <v>2227</v>
       </c>
       <c r="B53" s="0">
-        <v>47.807114675556761</v>
+        <v>50.724990086756982</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>2083</v>
+        <v>2228</v>
       </c>
       <c r="B54" s="0"/>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>2084</v>
+        <v>2229</v>
       </c>
       <c r="B55" s="0">
-        <v>0.013200717753390783</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>2085</v>
+        <v>2230</v>
       </c>
       <c r="B56" s="0">
-        <v>0.22404653438592209</v>
+        <v>0.0064496668899090073</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>2086</v>
+        <v>2231</v>
       </c>
       <c r="B57" s="0">
-        <v>1.3148822868167553</v>
+        <v>0.1399000592045655</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>2087</v>
+        <v>2232</v>
       </c>
       <c r="B58" s="0">
-        <v>12.786555498378227</v>
+        <v>5.367044768109122</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>2088</v>
+        <v>2233</v>
       </c>
       <c r="B59" s="0">
-        <v>12.83535746989258</v>
+        <v>12.297961729450003</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>2089</v>
+        <v>2234</v>
       </c>
       <c r="B60" s="0">
-        <v>15.054940606516276</v>
+        <v>25.700541188592656</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>2090</v>
+        <v>2235</v>
       </c>
       <c r="B61" s="0">
-        <v>26.270145372069717</v>
+        <v>44.644255476759525</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>2091</v>
+        <v>2236</v>
       </c>
       <c r="B62" s="0">
-        <v>30.059369242172899</v>
+        <v>509.85832466801475</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>2092</v>
+        <v>2237</v>
       </c>
       <c r="B63" s="0"/>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>2093</v>
+        <v>2238</v>
       </c>
       <c r="B64" s="0">
         <v>0</v>
@@ -7118,69 +7555,69 @@
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>2094</v>
+        <v>2239</v>
       </c>
       <c r="B65" s="0">
-        <v>0</v>
+        <v>0.00072039826915172253</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>2095</v>
+        <v>2240</v>
       </c>
       <c r="B66" s="0">
-        <v>0.049881959099853032</v>
+        <v>0.012662848290688854</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>2096</v>
+        <v>2241</v>
       </c>
       <c r="B67" s="0">
-        <v>1.168088384065751</v>
+        <v>0.8470104792726656</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>2097</v>
+        <v>2242</v>
       </c>
       <c r="B68" s="0">
-        <v>1.9791726905717764</v>
+        <v>1.8818297095162966</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>2098</v>
+        <v>2243</v>
       </c>
       <c r="B69" s="0">
-        <v>3.7582008717874227</v>
+        <v>5.4754832293668452</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>2099</v>
+        <v>2244</v>
       </c>
       <c r="B70" s="0">
-        <v>5.1382638184815619</v>
+        <v>9.3335554574626389</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>2100</v>
+        <v>2245</v>
       </c>
       <c r="B71" s="0">
-        <v>10.210418515428744</v>
+        <v>18.111643641245397</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>2101</v>
+        <v>2246</v>
       </c>
       <c r="B72" s="0"/>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>2102</v>
+        <v>2247</v>
       </c>
       <c r="B73" s="0">
         <v>0</v>
@@ -7188,7 +7625,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>2103</v>
+        <v>2248</v>
       </c>
       <c r="B74" s="0">
         <v>0</v>
@@ -7196,153 +7633,153 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>2104</v>
+        <v>2249</v>
       </c>
       <c r="B75" s="0">
-        <v>0</v>
+        <v>0.020029161079986715</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>2105</v>
+        <v>2250</v>
       </c>
       <c r="B76" s="0">
-        <v>6.5024545032956524</v>
+        <v>1.7985929381173993</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>2106</v>
+        <v>2251</v>
       </c>
       <c r="B77" s="0">
-        <v>8.9931608450129659</v>
+        <v>4.7342819551531381</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>2107</v>
+        <v>2252</v>
       </c>
       <c r="B78" s="0">
-        <v>11.812413233991226</v>
+        <v>12.22521450274523</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>2108</v>
+        <v>2253</v>
       </c>
       <c r="B79" s="0">
-        <v>13.06335406459238</v>
+        <v>25.903612407263296</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>2109</v>
+        <v>2254</v>
       </c>
       <c r="B80" s="0">
-        <v>24.44451824650675</v>
+        <v>477.73724131024335</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>2110</v>
+        <v>2255</v>
       </c>
       <c r="B81" s="0"/>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>2111</v>
+        <v>2256</v>
       </c>
       <c r="B82" s="0"/>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>2112</v>
+        <v>2257</v>
       </c>
       <c r="B83" s="0"/>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>2113</v>
+        <v>2258</v>
       </c>
       <c r="B84" s="0"/>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>2114</v>
+        <v>2259</v>
       </c>
       <c r="B85" s="0"/>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>2115</v>
+        <v>2260</v>
       </c>
       <c r="B86" s="0"/>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>2116</v>
+        <v>2261</v>
       </c>
       <c r="B87" s="0"/>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>2117</v>
+        <v>2262</v>
       </c>
       <c r="B88" s="0"/>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>2118</v>
+        <v>2263</v>
       </c>
       <c r="B89" s="0"/>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>2119</v>
+        <v>2264</v>
       </c>
       <c r="B90" s="0"/>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>2120</v>
+        <v>2265</v>
       </c>
       <c r="B91" s="0"/>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>2121</v>
+        <v>2266</v>
       </c>
       <c r="B92" s="0">
-        <v>1000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>2122</v>
+        <v>2267</v>
       </c>
       <c r="B93" s="0">
-        <v>1000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>2123</v>
+        <v>2268</v>
       </c>
       <c r="B94" s="0">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>2124</v>
+        <v>2269</v>
       </c>
       <c r="B95" s="0">
-        <v>9.9999999999999998e-13</v>
+        <v>1e-10</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>2125</v>
+        <v>2270</v>
       </c>
       <c r="B96" s="0">
         <v>0.0074480424928103682</v>
@@ -7350,7 +7787,7 @@
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>2126</v>
+        <v>2271</v>
       </c>
       <c r="B97" s="0">
         <v>0</v>
@@ -7358,7 +7795,7 @@
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>2127</v>
+        <v>2272</v>
       </c>
       <c r="B98" s="0">
         <v>0</v>
@@ -7366,7 +7803,7 @@
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>2128</v>
+        <v>2273</v>
       </c>
       <c r="B99" s="0">
         <v>0</v>
@@ -7374,71 +7811,73 @@
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>2129</v>
+        <v>2274</v>
       </c>
       <c r="B100" s="0"/>
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>2130</v>
+        <v>2275</v>
       </c>
       <c r="B101" s="0"/>
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>2131</v>
+        <v>2276</v>
       </c>
       <c r="B102" s="0"/>
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>2132</v>
+        <v>2277</v>
       </c>
       <c r="B103" s="0"/>
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>2133</v>
+        <v>2278</v>
       </c>
       <c r="B104" s="0"/>
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>2134</v>
+        <v>2279</v>
       </c>
       <c r="B105" s="0"/>
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>2135</v>
+        <v>2280</v>
       </c>
       <c r="B106" s="0"/>
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>2136</v>
-      </c>
-      <c r="B107" s="0"/>
+        <v>2281</v>
+      </c>
+      <c r="B107" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>2137</v>
+        <v>2282</v>
       </c>
       <c r="B108" s="0">
-        <v>0.0020773236596895272</v>
+        <v>0.0025000000000000001</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>2138</v>
+        <v>2283</v>
       </c>
       <c r="B109" s="0">
-        <v>0.0030000000000000001</v>
+        <v>0.029144683373296388</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>2139</v>
+        <v>2284</v>
       </c>
       <c r="B110" s="0">
         <v>0.0050000000000000001</v>
@@ -7446,7 +7885,7 @@
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>2140</v>
+        <v>2285</v>
       </c>
       <c r="B111" s="0" t="b">
         <v>0</v>
@@ -7454,7 +7893,7 @@
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>2141</v>
+        <v>2286</v>
       </c>
       <c r="B112" s="0">
         <v>20</v>
@@ -7462,7 +7901,7 @@
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>2142</v>
+        <v>2287</v>
       </c>
       <c r="B113" s="0">
         <v>500</v>
@@ -7470,7 +7909,7 @@
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>2143</v>
+        <v>2288</v>
       </c>
       <c r="B114" s="0">
         <v>0</v>
@@ -7478,7 +7917,7 @@
     </row>
     <row r="115">
       <c r="A115" s="0" t="s">
-        <v>2144</v>
+        <v>2289</v>
       </c>
       <c r="B115" s="0">
         <v>1</v>
@@ -7486,7 +7925,7 @@
     </row>
     <row r="116">
       <c r="A116" s="0" t="s">
-        <v>2145</v>
+        <v>2290</v>
       </c>
       <c r="B116" s="0">
         <v>67131.732999999993</v>
@@ -7494,208 +7933,208 @@
     </row>
     <row r="117">
       <c r="A117" s="0" t="s">
-        <v>2146</v>
+        <v>2291</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>2174</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="s">
-        <v>2147</v>
+        <v>2292</v>
       </c>
       <c r="B118" s="0"/>
     </row>
     <row r="119">
       <c r="A119" s="0" t="s">
-        <v>2148</v>
+        <v>2293</v>
       </c>
       <c r="B119" s="0">
-        <v>0.51223045202004069</v>
+        <v>0.36080005587301012</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="s">
-        <v>2149</v>
+        <v>2294</v>
       </c>
       <c r="B120" s="0">
-        <v>0.51328421275968772</v>
+        <v>0.37585604482981705</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="s">
-        <v>2150</v>
+        <v>2295</v>
       </c>
       <c r="B121" s="0">
-        <v>0.51436406958828651</v>
+        <v>0.3915304242986698</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="s">
-        <v>2151</v>
+        <v>2296</v>
       </c>
       <c r="B122" s="0">
-        <v>0.51658487145535148</v>
+        <v>0.42434758381541704</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="s">
-        <v>2152</v>
+        <v>2297</v>
       </c>
       <c r="B123" s="0">
-        <v>0.52342638170970945</v>
+        <v>0.52758438977026278</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="s">
-        <v>2153</v>
+        <v>2298</v>
       </c>
       <c r="B124" s="0">
-        <v>0.53336190747233603</v>
+        <v>0.66918430952549413</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="s">
-        <v>2154</v>
+        <v>2299</v>
       </c>
       <c r="B125" s="0">
-        <v>0.51380992601184727</v>
+        <v>0.38345908763941339</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="s">
-        <v>2155</v>
+        <v>2300</v>
       </c>
       <c r="B126" s="0">
-        <v>0.51544263391625855</v>
+        <v>0.40738523898396806</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="s">
-        <v>2156</v>
+        <v>2301</v>
       </c>
       <c r="B127" s="0">
-        <v>0.51881089938924119</v>
+        <v>0.45776049005366687</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="s">
-        <v>2157</v>
+        <v>2302</v>
       </c>
       <c r="B128" s="0">
-        <v>0.52871515579569972</v>
+        <v>0.60605844393791575</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="s">
-        <v>2158</v>
+        <v>2303</v>
       </c>
       <c r="B129" s="0">
-        <v>0.53855530675886076</v>
+        <v>0.70934131102150311</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="s">
-        <v>2159</v>
+        <v>2304</v>
       </c>
       <c r="B130" s="0">
-        <v>0.024207624860011785</v>
+        <v>0.10230574988439389</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="s">
-        <v>2160</v>
+        <v>2305</v>
       </c>
       <c r="B131" s="0">
-        <v>0.058151029926492181</v>
+        <v>0.21100195724016668</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="s">
-        <v>2161</v>
+        <v>2306</v>
       </c>
       <c r="B132" s="0">
-        <v>0.085156268608744534</v>
+        <v>0.2834653389134294</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="s">
-        <v>2162</v>
+        <v>2307</v>
       </c>
       <c r="B133" s="0">
-        <v>0.11573036985589466</v>
+        <v>0.29990235257826753</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="s">
-        <v>2163</v>
+        <v>2308</v>
       </c>
       <c r="B134" s="0">
-        <v>0.1842080455542438</v>
+        <v>0.32157126512711259</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="s">
-        <v>2164</v>
+        <v>2309</v>
       </c>
       <c r="B135" s="0">
-        <v>0.20696699758572265</v>
+        <v>0.34495587662675342</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="s">
-        <v>2165</v>
+        <v>2310</v>
       </c>
       <c r="B136" s="0">
-        <v>0.073144349889313162</v>
+        <v>0.25643440094530812</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="s">
-        <v>2166</v>
+        <v>2311</v>
       </c>
       <c r="B137" s="0">
-        <v>0.10060340058433585</v>
+        <v>0.29275270000629455</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="s">
-        <v>2167</v>
+        <v>2312</v>
       </c>
       <c r="B138" s="0">
-        <v>0.14220275134473714</v>
+        <v>0.31009615579546762</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="s">
-        <v>2168</v>
+        <v>2313</v>
       </c>
       <c r="B139" s="0">
-        <v>0.20663110085553599</v>
+        <v>0.3324495961910276</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="s">
-        <v>2169</v>
+        <v>2314</v>
       </c>
       <c r="B140" s="0">
-        <v>0.20780686716031577</v>
+        <v>0.51639890860726667</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="s">
-        <v>2170</v>
+        <v>2315</v>
       </c>
       <c r="B141" s="0">
-        <v>0.072769243675301243</v>
+        <v>0.28138856860208489</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="s">
-        <v>2171</v>
+        <v>2316</v>
       </c>
       <c r="B142" s="0">
-        <v>0.044652177826712006</v>
+        <v>0.21445419283055064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update combine runs batch with my CNET ID
</commit_message>
<xml_diff>
--- a/output/run1_table.xlsx
+++ b/output/run1_table.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2320" uniqueCount="2320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2465" uniqueCount="2465">
   <si>
     <t>Row</t>
   </si>
@@ -6535,6 +6535,441 @@
   </si>
   <si>
     <t>unnamed</t>
+  </si>
+  <si>
+    <t>cont_a, no meas err</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>beta (annualized)</t>
+  </si>
+  <si>
+    <t>____Income Statistics</t>
+  </si>
+  <si>
+    <t>Mean gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log gross annual income</t>
+  </si>
+  <si>
+    <t>Stdev log net annual income</t>
+  </si>
+  <si>
+    <t>____Wealth Statistics</t>
+  </si>
+  <si>
+    <t>Mean total wealth</t>
+  </si>
+  <si>
+    <t>Mean liquid wealth</t>
+  </si>
+  <si>
+    <t>w, median</t>
+  </si>
+  <si>
+    <t>b, median</t>
+  </si>
+  <si>
+    <t>s = 0</t>
+  </si>
+  <si>
+    <t>b &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= 15% mean ann inc</t>
+  </si>
+  <si>
+    <t>b &lt;= $500</t>
+  </si>
+  <si>
+    <t>b &lt;= $1000</t>
+  </si>
+  <si>
+    <t>b &lt;= $2000</t>
+  </si>
+  <si>
+    <t>b &lt;= $5000</t>
+  </si>
+  <si>
+    <t>b &lt;= $10000</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>b_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/6</t>
+  </si>
+  <si>
+    <t>P(WHtM) / P(HtM), HtM in terms of y/12</t>
+  </si>
+  <si>
+    <t>w, Top 10% share</t>
+  </si>
+  <si>
+    <t>w, Top 1% share</t>
+  </si>
+  <si>
+    <t>Gini coefficient, wealth</t>
+  </si>
+  <si>
+    <t>____MPC size effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____MPC sign effects</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Annual  MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>____MPC for HtM households</t>
+  </si>
+  <si>
+    <t>Quarterly  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  HtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  WHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual  PHtM MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>____Wealth percentiles</t>
+  </si>
+  <si>
+    <t>w, 10th pctile</t>
+  </si>
+  <si>
+    <t>w, 25th pctile</t>
+  </si>
+  <si>
+    <t>w, 50th pctile</t>
+  </si>
+  <si>
+    <t>w, 90th pctile</t>
+  </si>
+  <si>
+    <t>w, 95th pctile</t>
+  </si>
+  <si>
+    <t>w, 98th pctile</t>
+  </si>
+  <si>
+    <t>w, 99th pctile</t>
+  </si>
+  <si>
+    <t>w, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Liquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>b, 10th pctile</t>
+  </si>
+  <si>
+    <t>b, 25th pctile</t>
+  </si>
+  <si>
+    <t>b, 50th pctile</t>
+  </si>
+  <si>
+    <t>b, 90th pctile</t>
+  </si>
+  <si>
+    <t>b, 95th pctile</t>
+  </si>
+  <si>
+    <t>b, 98th pctile</t>
+  </si>
+  <si>
+    <t>b, 99th pctile</t>
+  </si>
+  <si>
+    <t>b, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid wealth percentiles</t>
+  </si>
+  <si>
+    <t>a, 10th pctile</t>
+  </si>
+  <si>
+    <t>a, 25th pctile</t>
+  </si>
+  <si>
+    <t>a, 50th pctile</t>
+  </si>
+  <si>
+    <t>a, 90th pctile</t>
+  </si>
+  <si>
+    <t>a, 95th pctile</t>
+  </si>
+  <si>
+    <t>a, 98th pctile</t>
+  </si>
+  <si>
+    <t>a, 99th pctile</t>
+  </si>
+  <si>
+    <t>a, 99.9th pctile</t>
+  </si>
+  <si>
+    <t>____Illiquid mpcs</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of -$5000</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Quarterly illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $1</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $500</t>
+  </si>
+  <si>
+    <t>Annual illiq MPC (%), out of $5000</t>
+  </si>
+  <si>
+    <t>____Adjustment cost statistics,cost(d,a) =k0 * |d| + k1 * |d| ^ (1 + k2) / (1 + k2)</t>
+  </si>
+  <si>
+    <t>kappa0, adj cost coeff on first (linear) term</t>
+  </si>
+  <si>
+    <t>kappa1, adj cost coeff on second (power) term</t>
+  </si>
+  <si>
+    <t>kappa2, power on second term</t>
+  </si>
+  <si>
+    <t>kappa1 ^(-1/kappa2), low values cause mass at high a</t>
+  </si>
+  <si>
+    <t>a_lb, parameter s.t. max(a, a_lb) used for adj cost</t>
+  </si>
+  <si>
+    <t>Mean adjustment cost, E[chi(d, a)]</t>
+  </si>
+  <si>
+    <t>Mean ratio of deposits to assets, E[|d| / max(a, a_lb)]</t>
+  </si>
+  <si>
+    <t>E[chi(d,a)/abs(d) | d != 0]</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 10th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 25th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 50th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 90th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 95th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>chi/abs(d), 99th pctile condl on d != 0</t>
+  </si>
+  <si>
+    <t>____Other parameters</t>
+  </si>
+  <si>
+    <t>Experiment group no.</t>
+  </si>
+  <si>
+    <t>Liquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Illiquid asset return (quarterly)</t>
+  </si>
+  <si>
+    <t>Death rate (quarterly)</t>
+  </si>
+  <si>
+    <t>Bequests, on or off</t>
+  </si>
+  <si>
+    <t>Max liquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Max illiquid assets, parameter</t>
+  </si>
+  <si>
+    <t>Borrowing limit</t>
+  </si>
+  <si>
+    <t>CRRA coefficient</t>
+  </si>
+  <si>
+    <t>Value of the numeraire, mean annual earning, in $</t>
+  </si>
+  <si>
+    <t>Income Process</t>
+  </si>
+  <si>
+    <t>____Other statistics</t>
+  </si>
+  <si>
+    <t>a &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>a &lt;= $500</t>
+  </si>
+  <si>
+    <t>a &lt;= $1000</t>
+  </si>
+  <si>
+    <t>a &lt;= $2000</t>
+  </si>
+  <si>
+    <t>a &lt;= $5000</t>
+  </si>
+  <si>
+    <t>a &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w &lt;= 0% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 0.5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 1% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 2% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 5% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= 10% mean ann inc</t>
+  </si>
+  <si>
+    <t>w &lt;= $500</t>
+  </si>
+  <si>
+    <t>w &lt;= $1000</t>
+  </si>
+  <si>
+    <t>w &lt;= $2000</t>
+  </si>
+  <si>
+    <t>w &lt;= $5000</t>
+  </si>
+  <si>
+    <t>w &lt;= $10000</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 6</t>
+  </si>
+  <si>
+    <t>w_i &lt;= y_i / 12</t>
+  </si>
+  <si>
+    <t>Specification1</t>
+  </si>
+  <si>
+    <t>cal=1, r_a=2.000000e-02, reb_cost=1.489608e-03</t>
   </si>
   <si>
     <t>cont_a, no meas err</t>
@@ -6993,7 +7428,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -7017,11 +7452,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -7039,6 +7475,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7057,53 +7494,53 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>2175</v>
+        <v>2320</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>2317</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>2176</v>
+        <v>2321</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2318</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2177</v>
+        <v>2322</v>
       </c>
       <c r="B3" s="0">
-        <v>16.797546998531971</v>
+        <v>16.797619060801473</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>2178</v>
+        <v>2323</v>
       </c>
       <c r="B4" s="0">
-        <v>40.643693986181724</v>
+        <v>40.643819048972794</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>2179</v>
+        <v>2324</v>
       </c>
       <c r="B5" s="0">
-        <v>0.92101277298502415</v>
+        <v>0.92101227701578969</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>2180</v>
+        <v>2325</v>
       </c>
       <c r="B6" s="0"/>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>2181</v>
+        <v>2326</v>
       </c>
       <c r="B7" s="0">
         <v>1.0991047620773315</v>
@@ -7111,7 +7548,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>2182</v>
+        <v>2327</v>
       </c>
       <c r="B8" s="0">
         <v>0.803355872631073</v>
@@ -7119,7 +7556,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>2183</v>
+        <v>2328</v>
       </c>
       <c r="B9" s="0">
         <v>0.803355872631073</v>
@@ -7127,357 +7564,357 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>2184</v>
+        <v>2329</v>
       </c>
       <c r="B10" s="0"/>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>2185</v>
+        <v>2330</v>
       </c>
       <c r="B11" s="0">
-        <v>4.0795939386802811</v>
+        <v>4.0796198957153385</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>2186</v>
+        <v>2331</v>
       </c>
       <c r="B12" s="0">
-        <v>0.56232947350128126</v>
+        <v>0.5623282670888563</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>2187</v>
+        <v>2332</v>
       </c>
       <c r="B13" s="0">
-        <v>0.1399000592045655</v>
+        <v>0.1398993580069407</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>2188</v>
+        <v>2333</v>
       </c>
       <c r="B14" s="0">
-        <v>0.012662848290688854</v>
+        <v>0.012662509800432651</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>2189</v>
+        <v>2334</v>
       </c>
       <c r="B15" s="0">
-        <v>0.40756267474146241</v>
+        <v>0.4075629552442579</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>2190</v>
+        <v>2335</v>
       </c>
       <c r="B16" s="0">
-        <v>0.16792334799990671</v>
+        <v>0.16792518131580744</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>2191</v>
+        <v>2336</v>
       </c>
       <c r="B17" s="0">
-        <v>0.35031682300309164</v>
+        <v>0.35031894208873854</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>2192</v>
+        <v>2337</v>
       </c>
       <c r="B18" s="0">
-        <v>0.47655635851259415</v>
+        <v>0.47655861970769453</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>2193</v>
+        <v>2338</v>
       </c>
       <c r="B19" s="0">
-        <v>0.53011351634723081</v>
+        <v>0.53011555643920438</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>2194</v>
+        <v>2339</v>
       </c>
       <c r="B20" s="0">
-        <v>0.61591168817242936</v>
+        <v>0.61591329492443425</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>2195</v>
+        <v>2340</v>
       </c>
       <c r="B21" s="0">
-        <v>0.67664470488462414</v>
+        <v>0.67664599083859067</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>2196</v>
+        <v>2341</v>
       </c>
       <c r="B22" s="0">
-        <v>0.7209766708036689</v>
+        <v>0.72097775007852705</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>2197</v>
+        <v>2342</v>
       </c>
       <c r="B23" s="0">
-        <v>0.42735848809702609</v>
+        <v>0.42736071810664678</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>2198</v>
+        <v>2343</v>
       </c>
       <c r="B24" s="0">
-        <v>0.50542783834144667</v>
+        <v>0.50542998745788981</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>2199</v>
+        <v>2344</v>
       </c>
       <c r="B25" s="0">
-        <v>0.56790660062105836</v>
+        <v>0.56790846371374359</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>2200</v>
+        <v>2345</v>
       </c>
       <c r="B26" s="0">
-        <v>0.64733699141370571</v>
+        <v>0.64733841479838938</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>2201</v>
+        <v>2346</v>
       </c>
       <c r="B27" s="0">
-        <v>0.72020753546714633</v>
+        <v>0.7202086182994164</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>2202</v>
+        <v>2347</v>
       </c>
       <c r="B28" s="0">
-        <v>0.50411046679164873</v>
+        <v>0.50411301118104845</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>2203</v>
+        <v>2348</v>
       </c>
       <c r="B29" s="0">
-        <v>0.40225260986085187</v>
+        <v>0.40225572507803248</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>2204</v>
+        <v>2349</v>
       </c>
       <c r="B30" s="0">
-        <v>0.44181169180447877</v>
+        <v>0.44181198341554062</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>2205</v>
+        <v>2350</v>
       </c>
       <c r="B31" s="0">
-        <v>0.46686687028647222</v>
+        <v>0.46686612599843746</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>2206</v>
+        <v>2351</v>
       </c>
       <c r="B32" s="0">
-        <v>0.86258896035485622</v>
+        <v>0.86259050832567696</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>2207</v>
+        <v>2352</v>
       </c>
       <c r="B33" s="0">
-        <v>0.57925496632296536</v>
+        <v>0.57925781619633954</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>2208</v>
+        <v>2353</v>
       </c>
       <c r="B34" s="0">
-        <v>0.911983421591268</v>
+        <v>0.91198429087108712</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>2209</v>
+        <v>2354</v>
       </c>
       <c r="B35" s="0"/>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>2210</v>
+        <v>2355</v>
       </c>
       <c r="B36" s="0">
-        <v>16.797546998525991</v>
+        <v>16.797619060800667</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>2211</v>
+        <v>2356</v>
       </c>
       <c r="B37" s="0">
-        <v>13.997199629235729</v>
+        <v>13.997276127853706</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>2212</v>
+        <v>2357</v>
       </c>
       <c r="B38" s="0">
-        <v>40.643693986158461</v>
+        <v>40.643819048966449</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>2213</v>
+        <v>2358</v>
       </c>
       <c r="B39" s="0">
-        <v>38.643388845311911</v>
+        <v>38.643551843952828</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>2214</v>
+        <v>2359</v>
       </c>
       <c r="B40" s="0"/>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>2215</v>
+        <v>2360</v>
       </c>
       <c r="B41" s="0">
-        <v>32.82006623527198</v>
+        <v>32.820231212924824</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>2216</v>
+        <v>2361</v>
       </c>
       <c r="B42" s="0">
-        <v>32.820066235285459</v>
+        <v>32.820231212924412</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>2217</v>
+        <v>2362</v>
       </c>
       <c r="B43" s="0">
-        <v>51.588456603163671</v>
+        <v>51.588670859431353</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>2218</v>
+        <v>2363</v>
       </c>
       <c r="B44" s="0">
-        <v>55.500440622710258</v>
+        <v>55.500575610506885</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>2219</v>
+        <v>2364</v>
       </c>
       <c r="B45" s="0">
-        <v>55.500440622698846</v>
+        <v>55.500575610512151</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>2220</v>
+        <v>2365</v>
       </c>
       <c r="B46" s="0">
-        <v>64.802849277509267</v>
+        <v>64.803048488296895</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>2221</v>
+        <v>2366</v>
       </c>
       <c r="B47" s="0"/>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>2222</v>
+        <v>2367</v>
       </c>
       <c r="B48" s="0">
-        <v>25.01515089267567</v>
+        <v>25.015182556551341</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>2223</v>
+        <v>2368</v>
       </c>
       <c r="B49" s="0">
-        <v>29.491861358078737</v>
+        <v>29.491931750983667</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>2224</v>
+        <v>2369</v>
       </c>
       <c r="B50" s="0">
-        <v>21.545251360383219</v>
+        <v>21.545248811330222</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>2225</v>
+        <v>2370</v>
       </c>
       <c r="B51" s="0">
-        <v>52.76044283642689</v>
+        <v>52.760489526418333</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>2226</v>
+        <v>2371</v>
       </c>
       <c r="B52" s="0">
-        <v>55.386493689334657</v>
+        <v>55.386670553946395</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>2227</v>
+        <v>2372</v>
       </c>
       <c r="B53" s="0">
-        <v>50.724990086756982</v>
+        <v>50.724933418023369</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>2228</v>
+        <v>2373</v>
       </c>
       <c r="B54" s="0"/>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>2229</v>
+        <v>2374</v>
       </c>
       <c r="B55" s="0">
         <v>0</v>
@@ -7485,69 +7922,69 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>2230</v>
+        <v>2375</v>
       </c>
       <c r="B56" s="0">
-        <v>0.0064496668899090073</v>
+        <v>0.0064495478887268889</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>2231</v>
+        <v>2376</v>
       </c>
       <c r="B57" s="0">
-        <v>0.1399000592045655</v>
+        <v>0.1398993580069407</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>2232</v>
+        <v>2377</v>
       </c>
       <c r="B58" s="0">
-        <v>5.367044768109122</v>
+        <v>5.3670428871992204</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>2233</v>
+        <v>2378</v>
       </c>
       <c r="B59" s="0">
-        <v>12.297961729450003</v>
+        <v>12.297966829244883</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>2234</v>
+        <v>2379</v>
       </c>
       <c r="B60" s="0">
-        <v>25.700541188592656</v>
+        <v>25.700593373471044</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>2235</v>
+        <v>2380</v>
       </c>
       <c r="B61" s="0">
-        <v>44.644255476759525</v>
+        <v>44.644663233045513</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>2236</v>
+        <v>2381</v>
       </c>
       <c r="B62" s="0">
-        <v>509.85832466801475</v>
+        <v>509.8584808568317</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>2237</v>
+        <v>2382</v>
       </c>
       <c r="B63" s="0"/>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>2238</v>
+        <v>2383</v>
       </c>
       <c r="B64" s="0">
         <v>0</v>
@@ -7555,69 +7992,69 @@
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>2239</v>
+        <v>2384</v>
       </c>
       <c r="B65" s="0">
-        <v>0.00072039826915172253</v>
+        <v>0.00072036252276311719</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>2240</v>
+        <v>2385</v>
       </c>
       <c r="B66" s="0">
-        <v>0.012662848290688854</v>
+        <v>0.012662509800432651</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>2241</v>
+        <v>2386</v>
       </c>
       <c r="B67" s="0">
-        <v>0.8470104792726656</v>
+        <v>0.84700670027597158</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>2242</v>
+        <v>2387</v>
       </c>
       <c r="B68" s="0">
-        <v>1.8818297095162966</v>
+        <v>1.8818244236781476</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>2243</v>
+        <v>2388</v>
       </c>
       <c r="B69" s="0">
-        <v>5.4754832293668452</v>
+        <v>5.4754841263080092</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>2244</v>
+        <v>2389</v>
       </c>
       <c r="B70" s="0">
-        <v>9.3335554574626389</v>
+        <v>9.3335654857998716</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>2245</v>
+        <v>2390</v>
       </c>
       <c r="B71" s="0">
-        <v>18.111643641245397</v>
+        <v>18.11165056771447</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>2246</v>
+        <v>2391</v>
       </c>
       <c r="B72" s="0"/>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>2247</v>
+        <v>2392</v>
       </c>
       <c r="B73" s="0">
         <v>0</v>
@@ -7625,7 +8062,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>2248</v>
+        <v>2393</v>
       </c>
       <c r="B74" s="0">
         <v>0</v>
@@ -7633,121 +8070,121 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>2249</v>
+        <v>2394</v>
       </c>
       <c r="B75" s="0">
-        <v>0.020029161079986715</v>
+        <v>0.020028874246319321</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>2250</v>
+        <v>2395</v>
       </c>
       <c r="B76" s="0">
-        <v>1.7985929381173993</v>
+        <v>1.7985885893610312</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>2251</v>
+        <v>2396</v>
       </c>
       <c r="B77" s="0">
-        <v>4.7342819551531381</v>
+        <v>4.7342834250513315</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>2252</v>
+        <v>2397</v>
       </c>
       <c r="B78" s="0">
-        <v>12.22521450274523</v>
+        <v>12.225254261609603</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>2253</v>
+        <v>2398</v>
       </c>
       <c r="B79" s="0">
-        <v>25.903612407263296</v>
+        <v>25.903830304905881</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>2254</v>
+        <v>2399</v>
       </c>
       <c r="B80" s="0">
-        <v>477.73724131024335</v>
+        <v>477.7379908452815</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>2255</v>
+        <v>2400</v>
       </c>
       <c r="B81" s="0"/>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>2256</v>
+        <v>2401</v>
       </c>
       <c r="B82" s="0"/>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>2257</v>
+        <v>2402</v>
       </c>
       <c r="B83" s="0"/>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>2258</v>
+        <v>2403</v>
       </c>
       <c r="B84" s="0"/>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>2259</v>
+        <v>2404</v>
       </c>
       <c r="B85" s="0"/>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>2260</v>
+        <v>2405</v>
       </c>
       <c r="B86" s="0"/>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>2261</v>
+        <v>2406</v>
       </c>
       <c r="B87" s="0"/>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>2262</v>
+        <v>2407</v>
       </c>
       <c r="B88" s="0"/>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>2263</v>
+        <v>2408</v>
       </c>
       <c r="B89" s="0"/>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>2264</v>
+        <v>2409</v>
       </c>
       <c r="B90" s="0"/>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>2265</v>
+        <v>2410</v>
       </c>
       <c r="B91" s="0"/>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>2266</v>
+        <v>2411</v>
       </c>
       <c r="B92" s="0">
         <v>10000000000</v>
@@ -7755,7 +8192,7 @@
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>2267</v>
+        <v>2412</v>
       </c>
       <c r="B93" s="0">
         <v>10000000000</v>
@@ -7763,7 +8200,7 @@
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>2268</v>
+        <v>2413</v>
       </c>
       <c r="B94" s="0">
         <v>1</v>
@@ -7771,7 +8208,7 @@
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>2269</v>
+        <v>2414</v>
       </c>
       <c r="B95" s="0">
         <v>1e-10</v>
@@ -7779,7 +8216,7 @@
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>2270</v>
+        <v>2415</v>
       </c>
       <c r="B96" s="0">
         <v>0.0074480424928103682</v>
@@ -7787,7 +8224,7 @@
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>2271</v>
+        <v>2416</v>
       </c>
       <c r="B97" s="0">
         <v>0</v>
@@ -7795,7 +8232,7 @@
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>2272</v>
+        <v>2417</v>
       </c>
       <c r="B98" s="0">
         <v>0</v>
@@ -7803,7 +8240,7 @@
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>2273</v>
+        <v>2418</v>
       </c>
       <c r="B99" s="0">
         <v>0</v>
@@ -7811,49 +8248,49 @@
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>2274</v>
+        <v>2419</v>
       </c>
       <c r="B100" s="0"/>
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>2275</v>
+        <v>2420</v>
       </c>
       <c r="B101" s="0"/>
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>2276</v>
+        <v>2421</v>
       </c>
       <c r="B102" s="0"/>
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>2277</v>
+        <v>2422</v>
       </c>
       <c r="B103" s="0"/>
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>2278</v>
+        <v>2423</v>
       </c>
       <c r="B104" s="0"/>
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>2279</v>
+        <v>2424</v>
       </c>
       <c r="B105" s="0"/>
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>2280</v>
+        <v>2425</v>
       </c>
       <c r="B106" s="0"/>
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>2281</v>
+        <v>2426</v>
       </c>
       <c r="B107" s="0">
         <v>1</v>
@@ -7861,7 +8298,7 @@
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>2282</v>
+        <v>2427</v>
       </c>
       <c r="B108" s="0">
         <v>0.0025000000000000001</v>
@@ -7869,15 +8306,15 @@
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>2283</v>
+        <v>2428</v>
       </c>
       <c r="B109" s="0">
-        <v>0.029144683373296388</v>
+        <v>0.029144842514776607</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>2284</v>
+        <v>2429</v>
       </c>
       <c r="B110" s="0">
         <v>0.0050000000000000001</v>
@@ -7885,7 +8322,7 @@
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>2285</v>
+        <v>2430</v>
       </c>
       <c r="B111" s="0" t="b">
         <v>0</v>
@@ -7893,7 +8330,7 @@
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>2286</v>
+        <v>2431</v>
       </c>
       <c r="B112" s="0">
         <v>20</v>
@@ -7901,7 +8338,7 @@
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>2287</v>
+        <v>2432</v>
       </c>
       <c r="B113" s="0">
         <v>500</v>
@@ -7909,7 +8346,7 @@
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>2288</v>
+        <v>2433</v>
       </c>
       <c r="B114" s="0">
         <v>0</v>
@@ -7917,7 +8354,7 @@
     </row>
     <row r="115">
       <c r="A115" s="0" t="s">
-        <v>2289</v>
+        <v>2434</v>
       </c>
       <c r="B115" s="0">
         <v>1</v>
@@ -7925,7 +8362,7 @@
     </row>
     <row r="116">
       <c r="A116" s="0" t="s">
-        <v>2290</v>
+        <v>2435</v>
       </c>
       <c r="B116" s="0">
         <v>67131.732999999993</v>
@@ -7933,208 +8370,208 @@
     </row>
     <row r="117">
       <c r="A117" s="0" t="s">
-        <v>2291</v>
+        <v>2436</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>2319</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="s">
-        <v>2292</v>
+        <v>2437</v>
       </c>
       <c r="B118" s="0"/>
     </row>
     <row r="119">
       <c r="A119" s="0" t="s">
-        <v>2293</v>
+        <v>2438</v>
       </c>
       <c r="B119" s="0">
-        <v>0.36080005587301012</v>
+        <v>0.36080110085715911</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="s">
-        <v>2294</v>
+        <v>2439</v>
       </c>
       <c r="B120" s="0">
-        <v>0.37585604482981705</v>
+        <v>0.3758570779629633</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="s">
-        <v>2295</v>
+        <v>2440</v>
       </c>
       <c r="B121" s="0">
-        <v>0.3915304242986698</v>
+        <v>0.39153144533962236</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="s">
-        <v>2296</v>
+        <v>2441</v>
       </c>
       <c r="B122" s="0">
-        <v>0.42434758381541704</v>
+        <v>0.4243485801140659</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="s">
-        <v>2297</v>
+        <v>2442</v>
       </c>
       <c r="B123" s="0">
-        <v>0.52758438977026278</v>
+        <v>0.52758531036049616</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="s">
-        <v>2298</v>
+        <v>2443</v>
       </c>
       <c r="B124" s="0">
-        <v>0.66918430952549413</v>
+        <v>0.66918511887551968</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="s">
-        <v>2299</v>
+        <v>2444</v>
       </c>
       <c r="B125" s="0">
-        <v>0.38345908763941339</v>
+        <v>0.38346011487968534</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="s">
-        <v>2300</v>
+        <v>2445</v>
       </c>
       <c r="B126" s="0">
-        <v>0.40738523898396806</v>
+        <v>0.40738624799016893</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="s">
-        <v>2301</v>
+        <v>2446</v>
       </c>
       <c r="B127" s="0">
-        <v>0.45776049005366687</v>
+        <v>0.45776146166869613</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="s">
-        <v>2302</v>
+        <v>2447</v>
       </c>
       <c r="B128" s="0">
-        <v>0.60605844393791575</v>
+        <v>0.60605930585114676</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="s">
-        <v>2303</v>
+        <v>2448</v>
       </c>
       <c r="B129" s="0">
-        <v>0.70934131102150311</v>
+        <v>0.70934205602833167</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="s">
-        <v>2304</v>
+        <v>2449</v>
       </c>
       <c r="B130" s="0">
-        <v>0.10230574988439389</v>
+        <v>0.1023071207498235</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="s">
-        <v>2305</v>
+        <v>2450</v>
       </c>
       <c r="B131" s="0">
-        <v>0.21100195724016668</v>
+        <v>0.21100319418946367</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="s">
-        <v>2306</v>
+        <v>2451</v>
       </c>
       <c r="B132" s="0">
-        <v>0.2834653389134294</v>
+        <v>0.28346648437526623</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="s">
-        <v>2307</v>
+        <v>2452</v>
       </c>
       <c r="B133" s="0">
-        <v>0.29990235257826753</v>
+        <v>0.29990346189605949</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="s">
-        <v>2308</v>
+        <v>2453</v>
       </c>
       <c r="B134" s="0">
-        <v>0.32157126512711259</v>
+        <v>0.32157229909126533</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="s">
-        <v>2309</v>
+        <v>2454</v>
       </c>
       <c r="B135" s="0">
-        <v>0.34495587662675342</v>
+        <v>0.34495698371241407</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="s">
-        <v>2310</v>
+        <v>2455</v>
       </c>
       <c r="B136" s="0">
-        <v>0.25643440094530812</v>
+        <v>0.25643558154233836</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="s">
-        <v>2311</v>
+        <v>2456</v>
       </c>
       <c r="B137" s="0">
-        <v>0.29275270000629455</v>
+        <v>0.29275382688363927</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="s">
-        <v>2312</v>
+        <v>2457</v>
       </c>
       <c r="B138" s="0">
-        <v>0.31009615579546762</v>
+        <v>0.31009723416494078</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="s">
-        <v>2313</v>
+        <v>2458</v>
       </c>
       <c r="B139" s="0">
-        <v>0.3324495961910276</v>
+        <v>0.33245063408502085</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="s">
-        <v>2314</v>
+        <v>2459</v>
       </c>
       <c r="B140" s="0">
-        <v>0.51639890860726667</v>
+        <v>0.516400636862135</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="s">
-        <v>2315</v>
+        <v>2460</v>
       </c>
       <c r="B141" s="0">
-        <v>0.28138856860208489</v>
+        <v>0.28138984184556881</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="s">
-        <v>2316</v>
+        <v>2461</v>
       </c>
       <c r="B142" s="0">
-        <v>0.21445419283055064</v>
+        <v>0.21445615305015894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>